<commit_message>
add right graph for inception 10gbps, in rack, even, no striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_even_nostriping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/10gbps_inrack_even_nostriping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.8055</c:v>
+                    <c:v>11.9524</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.5635</c:v>
+                    <c:v>9.1992</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.5977</c:v>
+                    <c:v>3.478</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5762</c:v>
+                    <c:v>5.873</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8539</c:v>
+                    <c:v>7.6531</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1643</c:v>
+                    <c:v>13.5974</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.0853</c:v>
+                    <c:v>11.0262</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.8491</c:v>
+                    <c:v>10.1916</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.1251</c:v>
+                    <c:v>1.6209</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>14.9473</c:v>
+                    <c:v>7.7476</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.4027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.7512</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9988</c:v>
+                  <c:v>-1.0402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0606</c:v>
+                  <c:v>0.1312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>7.6142</c:v>
+                    <c:v>4.2388</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8392</c:v>
+                    <c:v>6.01</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.7893</c:v>
+                    <c:v>6.4428</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.3474</c:v>
+                    <c:v>2.0983</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>16.8722</c:v>
+                    <c:v>4.1915</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>6.0461</c:v>
+                    <c:v>4.508</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.3747</c:v>
+                    <c:v>4.5455</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>24.1937</c:v>
+                    <c:v>5.9731</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.137</c:v>
+                    <c:v>6.7045</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.7235</c:v>
+                    <c:v>2.4735</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-1.5776</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>2.1995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.476</c:v>
+                  <c:v>-1.752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4679</c:v>
+                  <c:v>5.7029</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3096</c:v>
+                  <c:v>0.0563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.3796</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.9703</c:v>
+                    <c:v>1.7996</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>12.2194</c:v>
+                    <c:v>5.705599999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>24.9427</c:v>
+                    <c:v>14.6106</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>23.1308</c:v>
+                    <c:v>11.1108</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.717</c:v>
+                    <c:v>3.7944</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>8.215</c:v>
+                    <c:v>3.9854</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4249</c:v>
+                    <c:v>1.7001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>61.4333</c:v>
+                    <c:v>13.3551</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>42.6265</c:v>
+                    <c:v>27.2555</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>1.0004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2533</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.3613</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.4249</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.2307</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.1762</c:v>
+                  <c:v>-3.7028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.3216</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.6137</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.032</c:v>
+                    <c:v>1.2486</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>50.4649</c:v>
+                    <c:v>35.7099</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>23.3337</c:v>
+                    <c:v>3.906</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.9496</c:v>
+                    <c:v>2.4255</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6688</c:v>
+                    <c:v>1.509</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.8899</c:v>
+                    <c:v>1.9189</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>63.306</c:v>
+                    <c:v>4.092</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>11.662</c:v>
+                    <c:v>8.2458</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.7627</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.7207</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4583</c:v>
+                  <c:v>0.7514</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.6879</c:v>
+                  <c:v>2.7016</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.8727</c:v>
+                  <c:v>1.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2057948512"/>
-        <c:axId val="-2057942256"/>
+        <c:axId val="-2074167440"/>
+        <c:axId val="-2074159376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2057948512"/>
+        <c:axId val="-2074167440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057942256"/>
+        <c:crossAx val="-2074159376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2057942256"/>
+        <c:axId val="-2074159376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057948512"/>
+        <c:crossAx val="-2074167440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2171</c:v>
+                    <c:v>2.3259</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.1705</c:v>
+                    <c:v>1.8367</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.0812</c:v>
+                    <c:v>3.4525</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.652</c:v>
+                    <c:v>3.2963</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0156</c:v>
+                    <c:v>4.1786</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.8877</c:v>
+                    <c:v>11.9524</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>9.8062</c:v>
+                    <c:v>8.9684</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.7254</c:v>
+                    <c:v>0.9043</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9481</c:v>
+                    <c:v>0.7994</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.7187</c:v>
+                    <c:v>2.394</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.2614</c:v>
+                  <c:v>11.9524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6969</c:v>
+                  <c:v>30.2282</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.6499</c:v>
+                  <c:v>26.2316</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.2293</c:v>
+                  <c:v>21.8395</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.5162</c:v>
+                  <c:v>18.7867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.5902</c:v>
+                    <c:v>4.3269</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5435</c:v>
+                    <c:v>2.8044</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7957</c:v>
+                    <c:v>4.9793</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.2417</c:v>
+                    <c:v>2.9344</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>18.3616</c:v>
+                    <c:v>2.2133</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>5.6442</c:v>
+                    <c:v>0.6157</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>12.8005</c:v>
+                    <c:v>4.6709</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>15.8614</c:v>
+                    <c:v>9.1443</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>22.7007</c:v>
+                    <c:v>24.208</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0969</c:v>
+                    <c:v>3.0456</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.6442</c:v>
+                  <c:v>3.3712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8473</c:v>
+                  <c:v>16.2321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.4547</c:v>
+                  <c:v>30.2139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0514</c:v>
+                  <c:v>31.5865</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.5762</c:v>
+                  <c:v>24.0315</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>2.2035</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.8839</c:v>
+                    <c:v>2.771</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.9446</c:v>
+                    <c:v>4.622</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>26.6162</c:v>
+                    <c:v>12.0635</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>18.257</c:v>
+                    <c:v>3.7273</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.3629</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>2.4821</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.3001</c:v>
+                    <c:v>2.5268</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>19.6544</c:v>
+                    <c:v>6.6895</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>27.8366</c:v>
+                    <c:v>1.7428</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1673,19 +1670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.7599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>7.5477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.8827</c:v>
+                  <c:v>15.0536</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.3573</c:v>
+                  <c:v>30.5002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.1588</c:v>
+                  <c:v>31.7077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>2.1348</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7171</c:v>
+                    <c:v>1.5711</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.662</c:v>
+                    <c:v>1.4433</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>44.1951</c:v>
+                    <c:v>37.6652</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>32.2425</c:v>
+                    <c:v>10.0808</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.3398</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>1.0542</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.5735</c:v>
+                    <c:v>1.9594</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.9918</c:v>
+                    <c:v>94.3064</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.7801</c:v>
+                    <c:v>46.5414</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1820,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>3.4208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.9955</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5735</c:v>
+                  <c:v>6.646899999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.4705</c:v>
+                  <c:v>15.8381</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.7015</c:v>
+                  <c:v>24.3243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2057866224"/>
-        <c:axId val="-2057859968"/>
+        <c:axId val="-2074886240"/>
+        <c:axId val="-2074892496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2057866224"/>
+        <c:axId val="-2074886240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057859968"/>
+        <c:crossAx val="-2074892496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2057859968"/>
+        <c:axId val="-2074892496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057866224"/>
+        <c:crossAx val="-2074886240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2171</c:v>
+                    <c:v>2.3432</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.923</c:v>
+                    <c:v>2.783</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.5264</c:v>
+                    <c:v>3.8234</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.874</c:v>
+                    <c:v>1.8925</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2307</c:v>
+                    <c:v>4.7367</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.8877</c:v>
+                    <c:v>11.9524</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>11.436</c:v>
+                    <c:v>9.1116</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.5741</c:v>
+                    <c:v>5.4191</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5555</c:v>
+                    <c:v>5.7814</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.865</c:v>
+                    <c:v>10.6545</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.2614</c:v>
+                  <c:v>11.9524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.3267</c:v>
+                  <c:v>30.3714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.0</c:v>
+                  <c:v>48.3671</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.0037</c:v>
+                  <c:v>65.147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.8463</c:v>
+                  <c:v>76.60509999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.5902</c:v>
+                    <c:v>4.3269</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5435</c:v>
+                    <c:v>2.8044</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7957</c:v>
+                    <c:v>4.9793</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.3003</c:v>
+                    <c:v>9.2433</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.1168</c:v>
+                    <c:v>2.006</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>5.6442</c:v>
+                    <c:v>0.6157</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>12.8005</c:v>
+                    <c:v>4.6709</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>15.8614</c:v>
+                    <c:v>9.1443</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.0109</c:v>
+                    <c:v>13.8184</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>14.9021</c:v>
+                    <c:v>22.4768</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.6442</c:v>
+                  <c:v>3.3712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.8473</c:v>
+                  <c:v>16.2321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.4547</c:v>
+                  <c:v>30.2139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.174</c:v>
+                  <c:v>45.3925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61.3106</c:v>
+                  <c:v>64.80549999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>2.2035</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.8839</c:v>
+                    <c:v>2.771</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.9446</c:v>
+                    <c:v>4.622</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>16.1105</c:v>
+                    <c:v>8.8798</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>16.8432</c:v>
+                    <c:v>5.2335</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.3629</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>2.4821</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.3001</c:v>
+                    <c:v>2.5268</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>23.739</c:v>
+                    <c:v>8.8233</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>33.0019</c:v>
+                    <c:v>33.578</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2705,19 +2702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>2.7599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>7.5477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.8827</c:v>
+                  <c:v>15.0536</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26.5239</c:v>
+                  <c:v>30.5002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.4433</c:v>
+                  <c:v>44.0283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>2.1348</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7171</c:v>
+                    <c:v>1.5711</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>3.662</c:v>
+                    <c:v>1.4433</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>49.9315</c:v>
+                    <c:v>40.6553</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>24.596</c:v>
+                    <c:v>3.6023</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>1.3398</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>1.0542</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.5735</c:v>
+                    <c:v>1.9594</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.4939</c:v>
+                    <c:v>12.3911</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>6.7023</c:v>
+                    <c:v>27.0283</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>3.4208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.9955</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5735</c:v>
+                  <c:v>6.646899999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6222</c:v>
+                  <c:v>15.9907</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.2917</c:v>
+                  <c:v>29.731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2057784336"/>
-        <c:axId val="-2057778080"/>
+        <c:axId val="-2073456208"/>
+        <c:axId val="-2073449952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2057784336"/>
+        <c:axId val="-2073456208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057778080"/>
+        <c:crossAx val="-2073449952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2057778080"/>
+        <c:axId val="-2073449952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057784336"/>
+        <c:crossAx val="-2073456208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3357,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0202</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.9343</c:v>
+                    <c:v>4.1939</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.7646</c:v>
+                    <c:v>6.9352</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.4715</c:v>
+                    <c:v>1.2807</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8813</c:v>
+                    <c:v>3.7614</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3387,13 +3384,13 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>4.4432</c:v>
+                    <c:v>7.465</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.7824</c:v>
+                    <c:v>7.4314</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.8057</c:v>
+                    <c:v>13.721</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3449,13 +3446,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.0684</c:v>
+                  <c:v>28.2545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.4985</c:v>
+                  <c:v>55.443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.5587</c:v>
+                  <c:v>72.0181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3513,10 +3510,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>9.198</c:v>
+                    <c:v>9.559</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2712</c:v>
+                    <c:v>0.4681</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3537,10 +3534,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.5688</c:v>
+                    <c:v>27.964</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>16.9374</c:v>
+                    <c:v>31.3727</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3599,10 +3596,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.6915</c:v>
+                  <c:v>24.5938</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.7214</c:v>
+                  <c:v>55.458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3660,10 +3657,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>21.9106</c:v>
+                    <c:v>16.6622</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>22.6949</c:v>
+                    <c:v>8.097300000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3684,10 +3681,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.8122</c:v>
+                    <c:v>10.2683</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>42.1678</c:v>
+                    <c:v>46.9374</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3746,10 +3743,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9197</c:v>
+                  <c:v>-1.2281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.4761</c:v>
+                  <c:v>15.8103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,10 +3804,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>8.2644</c:v>
+                    <c:v>53.2565</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>24.3257</c:v>
+                    <c:v>42.9981</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3831,10 +3828,10 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.4145</c:v>
+                    <c:v>1.7988</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.9635</c:v>
+                    <c:v>28.078</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3893,10 +3890,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3119</c:v>
+                  <c:v>-0.3289</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1547</c:v>
+                  <c:v>-0.4934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2057704192"/>
-        <c:axId val="-2057697936"/>
+        <c:axId val="-2073349568"/>
+        <c:axId val="-2073343312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2057704192"/>
+        <c:axId val="-2073349568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057697936"/>
+        <c:crossAx val="-2073343312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2057697936"/>
+        <c:axId val="-2073343312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057704192"/>
+        <c:crossAx val="-2073349568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>1.0911999999999999</v>
-          </cell>
-          <cell r="G4">
-            <v>1.0779000000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>1.2456</v>
-          </cell>
-          <cell r="F5">
-            <v>1.407</v>
-          </cell>
-          <cell r="G5">
-            <v>0.99739999999999995</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>16.129000000000001</v>
-          </cell>
-          <cell r="F6">
-            <v>3.9912999999999998</v>
-          </cell>
-          <cell r="G6">
-            <v>4.5518999999999998</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>28.493200000000002</v>
-          </cell>
-          <cell r="F7">
-            <v>12.5747</v>
-          </cell>
-          <cell r="G7">
-            <v>2.8045</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>36.925699999999999</v>
-          </cell>
-          <cell r="F8">
-            <v>7.7286999999999999</v>
-          </cell>
-          <cell r="G8">
-            <v>1.1873</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-          <cell r="F10">
-            <v>0</v>
-          </cell>
-          <cell r="G10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>0</v>
-          </cell>
-          <cell r="G11">
-            <v>3.3603000000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>17.674199999999999</v>
-          </cell>
-          <cell r="F12">
-            <v>4.8032000000000004</v>
-          </cell>
-          <cell r="G12">
-            <v>4.5731999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>29.992100000000001</v>
-          </cell>
-          <cell r="F13">
-            <v>26.671199999999999</v>
-          </cell>
-          <cell r="G13">
-            <v>2.1979000000000002</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>37.325299999999999</v>
-          </cell>
-          <cell r="F14">
-            <v>3.5363000000000002</v>
-          </cell>
-          <cell r="G14">
-            <v>0.55710000000000004</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>0</v>
-          </cell>
-          <cell r="G16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>2.0400000000000001E-2</v>
-          </cell>
-          <cell r="G17">
-            <v>2.0500000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>0</v>
-          </cell>
-          <cell r="F18">
-            <v>0</v>
-          </cell>
-          <cell r="G18">
-            <v>7.585</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>18.0519</v>
-          </cell>
-          <cell r="F19">
-            <v>1.6042000000000001</v>
-          </cell>
-          <cell r="G19">
-            <v>3.2688999999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>32.878100000000003</v>
-          </cell>
-          <cell r="F20">
-            <v>11.919</v>
-          </cell>
-          <cell r="G20">
-            <v>2.7446000000000002</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>0.3196</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>0</v>
-          </cell>
-          <cell r="F24">
-            <v>0</v>
-          </cell>
-          <cell r="G24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-1.3866000000000001</v>
-          </cell>
-          <cell r="F25">
-            <v>9.5091000000000001</v>
-          </cell>
-          <cell r="G25">
-            <v>13.7889</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>20.470700000000001</v>
-          </cell>
-          <cell r="F26">
-            <v>44.099600000000002</v>
-          </cell>
-          <cell r="G26">
-            <v>15.2531</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>11.7545</v>
-          </cell>
-          <cell r="F29">
-            <v>1.3320000000000001</v>
-          </cell>
-          <cell r="G29">
-            <v>1.724</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>9.9132999999999996</v>
-          </cell>
-          <cell r="F30">
-            <v>1.7428999999999999</v>
-          </cell>
-          <cell r="G30">
-            <v>1.355</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>29.48</v>
-          </cell>
-          <cell r="F31">
-            <v>0.44230000000000003</v>
-          </cell>
-          <cell r="G31">
-            <v>0.60260000000000002</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>39.526699999999998</v>
-          </cell>
-          <cell r="F32">
-            <v>0.69899999999999995</v>
-          </cell>
-          <cell r="G32">
-            <v>1.5249999999999999</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>45.844299999999997</v>
-          </cell>
-          <cell r="F33">
-            <v>0.89900000000000002</v>
-          </cell>
-          <cell r="G33">
-            <v>0.51139999999999997</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>13.3262</v>
-          </cell>
-          <cell r="F35">
-            <v>1.4916</v>
-          </cell>
-          <cell r="G35">
-            <v>0.68930000000000002</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>13.0052</v>
-          </cell>
-          <cell r="F36">
-            <v>1.5077</v>
-          </cell>
-          <cell r="G36">
-            <v>0.1249</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>34.027099999999997</v>
-          </cell>
-          <cell r="F37">
-            <v>0.56200000000000006</v>
-          </cell>
-          <cell r="G37">
-            <v>0.77129999999999999</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>44.891300000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>1.9685999999999999</v>
-          </cell>
-          <cell r="G38">
-            <v>0.78090000000000004</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>49.067</v>
-          </cell>
-          <cell r="F39">
-            <v>0.48970000000000002</v>
-          </cell>
-          <cell r="G39">
-            <v>1.5214000000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>1.4333</v>
-          </cell>
-          <cell r="F41">
-            <v>0.1797</v>
-          </cell>
-          <cell r="G41">
-            <v>8.4900000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>-14.854100000000001</v>
-          </cell>
-          <cell r="F42">
-            <v>0.83220000000000005</v>
-          </cell>
-          <cell r="G42">
-            <v>2.2370000000000001</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>15.901400000000001</v>
-          </cell>
-          <cell r="F43">
-            <v>0.60099999999999998</v>
-          </cell>
-          <cell r="G43">
-            <v>0.59899999999999998</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>34.833199999999998</v>
-          </cell>
-          <cell r="F44">
-            <v>3.4192999999999998</v>
-          </cell>
-          <cell r="G44">
-            <v>0.62690000000000001</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>44.505499999999998</v>
-          </cell>
-          <cell r="F45">
-            <v>0.72640000000000005</v>
-          </cell>
-          <cell r="G45">
-            <v>0.4834</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>2.5449999999999999</v>
-          </cell>
-          <cell r="F48">
-            <v>0.32979999999999998</v>
-          </cell>
-          <cell r="G48">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>-10.950100000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>0.89039999999999997</v>
-          </cell>
-          <cell r="G49">
-            <v>0.83489999999999998</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>16.394300000000001</v>
-          </cell>
-          <cell r="F50">
-            <v>54.334499999999998</v>
-          </cell>
-          <cell r="G50">
-            <v>16.245100000000001</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>36.4</v>
-          </cell>
-          <cell r="F51">
-            <v>24.002400000000002</v>
-          </cell>
-          <cell r="G51">
-            <v>13.4595</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>11.7545</v>
-          </cell>
-          <cell r="F54">
-            <v>1.3320000000000001</v>
-          </cell>
-          <cell r="G54">
-            <v>1.724</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>10.0258</v>
-          </cell>
-          <cell r="F55">
-            <v>1.0678000000000001</v>
-          </cell>
-          <cell r="G55">
-            <v>1.7574000000000001</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>48.6616</v>
-          </cell>
-          <cell r="F56">
-            <v>4.6632999999999996</v>
-          </cell>
-          <cell r="G56">
-            <v>4.3293999999999997</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>72.901899999999998</v>
-          </cell>
-          <cell r="F57">
-            <v>17.129000000000001</v>
-          </cell>
-          <cell r="G57">
-            <v>2.3666999999999998</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>86.078199999999995</v>
-          </cell>
-          <cell r="F58">
-            <v>5.3712</v>
-          </cell>
-          <cell r="G58">
-            <v>1.7237</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>13.3262</v>
-          </cell>
-          <cell r="F60">
-            <v>1.4916</v>
-          </cell>
-          <cell r="G60">
-            <v>0.68930000000000002</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>13.0253</v>
-          </cell>
-          <cell r="F61">
-            <v>1.5278</v>
-          </cell>
-          <cell r="G61">
-            <v>3.4495</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>51.950099999999999</v>
-          </cell>
-          <cell r="F62">
-            <v>4.2807000000000004</v>
-          </cell>
-          <cell r="G62">
-            <v>3.9687000000000001</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>75.480199999999996</v>
-          </cell>
-          <cell r="F63">
-            <v>5.0841000000000003</v>
-          </cell>
-          <cell r="G63">
-            <v>0.93200000000000005</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>87.154899999999998</v>
-          </cell>
-          <cell r="F64">
-            <v>13.6145</v>
-          </cell>
-          <cell r="G64">
-            <v>5.8700000000000002E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>1.4333</v>
-          </cell>
-          <cell r="F66">
-            <v>0.1797</v>
-          </cell>
-          <cell r="G66">
-            <v>8.4900000000000003E-2</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>-14.854100000000001</v>
-          </cell>
-          <cell r="F67">
-            <v>0.83220000000000005</v>
-          </cell>
-          <cell r="G67">
-            <v>2.2370000000000001</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>16.253599999999999</v>
-          </cell>
-          <cell r="F68">
-            <v>0.95320000000000005</v>
-          </cell>
-          <cell r="G68">
-            <v>7.2328000000000001</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>54.555500000000002</v>
-          </cell>
-          <cell r="F69">
-            <v>6.726</v>
-          </cell>
-          <cell r="G69">
-            <v>3.8308</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>77.211399999999998</v>
-          </cell>
-          <cell r="F70">
-            <v>2.6758999999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>0.42659999999999998</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>2.5449999999999999</v>
-          </cell>
-          <cell r="F73">
-            <v>0.32979999999999998</v>
-          </cell>
-          <cell r="G73">
-            <v>0.12</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>-10.950100000000001</v>
-          </cell>
-          <cell r="F74">
-            <v>0.89039999999999997</v>
-          </cell>
-          <cell r="G74">
-            <v>0.83489999999999998</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>18.454599999999999</v>
-          </cell>
-          <cell r="F75">
-            <v>4.1291000000000002</v>
-          </cell>
-          <cell r="G75">
-            <v>10.368399999999999</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>56.583799999999997</v>
-          </cell>
-          <cell r="F76">
-            <v>13.653700000000001</v>
-          </cell>
-          <cell r="G76">
-            <v>8.9168000000000003</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>0</v>
-          </cell>
-          <cell r="F80">
-            <v>0</v>
-          </cell>
-          <cell r="G80">
-            <v>3.9342999999999999</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>27.0684</v>
-          </cell>
-          <cell r="F81">
-            <v>7.1654</v>
-          </cell>
-          <cell r="G81">
-            <v>6.6866000000000003</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>55.046999999999997</v>
-          </cell>
-          <cell r="F82">
-            <v>28.687000000000001</v>
-          </cell>
-          <cell r="G82">
-            <v>4.4339000000000004</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>74.048000000000002</v>
-          </cell>
-          <cell r="F83">
-            <v>9.0913000000000004</v>
-          </cell>
-          <cell r="G83">
-            <v>3.4348000000000001</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>3.8502999999999998</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>26.8826</v>
-          </cell>
-          <cell r="F87">
-            <v>7.1422999999999996</v>
-          </cell>
-          <cell r="G87">
-            <v>6.6585999999999999</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>56.129899999999999</v>
-          </cell>
-          <cell r="F88">
-            <v>8.9312000000000005</v>
-          </cell>
-          <cell r="G88">
-            <v>0.91120000000000001</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>74.415499999999994</v>
-          </cell>
-          <cell r="F89">
-            <v>26.265499999999999</v>
-          </cell>
-          <cell r="G89">
-            <v>0.64980000000000004</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>0</v>
-          </cell>
-          <cell r="F93">
-            <v>0</v>
-          </cell>
-          <cell r="G93">
-            <v>9.0191999999999997</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>30.857199999999999</v>
-          </cell>
-          <cell r="F94">
-            <v>7.4958999999999998</v>
-          </cell>
-          <cell r="G94">
-            <v>4.9538000000000002</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>58.700400000000002</v>
-          </cell>
-          <cell r="F95">
-            <v>3.9940000000000002</v>
-          </cell>
-          <cell r="G95">
-            <v>1.3427</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>1.8240000000000001</v>
-          </cell>
-          <cell r="F100">
-            <v>8.5667000000000009</v>
-          </cell>
-          <cell r="G100">
-            <v>38.8934</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>31.768999999999998</v>
-          </cell>
-          <cell r="F101">
-            <v>21.7742</v>
-          </cell>
-          <cell r="G101">
-            <v>11.7645</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6874,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,10 +6941,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1643</v>
+        <v>13.5974</v>
       </c>
       <c r="G4">
-        <v>2.8054999999999999</v>
+        <v>11.952400000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.4027</v>
       </c>
       <c r="F5">
-        <v>5.0853000000000002</v>
+        <v>11.026199999999999</v>
       </c>
       <c r="G5">
-        <v>1.5634999999999999</v>
+        <v>9.1991999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6984,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-0.75119999999999998</v>
       </c>
       <c r="F6">
-        <v>3.8491</v>
+        <v>10.191599999999999</v>
       </c>
       <c r="G6">
-        <v>4.5976999999999997</v>
+        <v>3.4780000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>0.99880000000000002</v>
+        <v>-1.0402</v>
       </c>
       <c r="F7">
-        <v>1.1251</v>
+        <v>1.6209</v>
       </c>
       <c r="G7">
-        <v>1.5762</v>
+        <v>5.8730000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>-1.0606</v>
+        <v>0.13120000000000001</v>
       </c>
       <c r="F8">
-        <v>14.9473</v>
+        <v>7.7476000000000003</v>
       </c>
       <c r="G8">
-        <v>0.85389999999999999</v>
+        <v>7.6531000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>-1.5775999999999999</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>6.0461</v>
+        <v>4.508</v>
       </c>
       <c r="G10">
-        <v>7.6142000000000003</v>
+        <v>4.2388000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7988,13 +7076,13 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2.1995</v>
       </c>
       <c r="F11">
-        <v>6.3746999999999998</v>
+        <v>4.5454999999999997</v>
       </c>
       <c r="G11">
-        <v>4.8391999999999999</v>
+        <v>6.01</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>0.47599999999999998</v>
+        <v>-1.752</v>
       </c>
       <c r="F12">
-        <v>24.1937</v>
+        <v>5.9730999999999996</v>
       </c>
       <c r="G12">
-        <v>4.7892999999999999</v>
+        <v>6.4428000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>2.4679000000000002</v>
+        <v>5.7028999999999996</v>
       </c>
       <c r="F13">
-        <v>7.1369999999999996</v>
+        <v>6.7045000000000003</v>
       </c>
       <c r="G13">
-        <v>3.3473999999999999</v>
+        <v>2.0983000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>3.3096000000000001</v>
+        <v>5.6300000000000003E-2</v>
       </c>
       <c r="F14">
-        <v>4.7234999999999996</v>
+        <v>2.4735</v>
       </c>
       <c r="G14">
-        <v>16.872199999999999</v>
+        <v>4.1914999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,13 +7168,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1.0004</v>
       </c>
       <c r="F16">
-        <v>3.7170000000000001</v>
+        <v>3.7944</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.37959999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8103,13 +7191,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>-1.3613</v>
+        <v>1.8379000000000001</v>
       </c>
       <c r="F17">
-        <v>8.2149999999999999</v>
+        <v>3.9853999999999998</v>
       </c>
       <c r="G17">
-        <v>4.9702999999999999</v>
+        <v>1.7996000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>0.4249</v>
+        <v>-1.2533000000000001</v>
       </c>
       <c r="F18">
-        <v>0.4249</v>
+        <v>1.7000999999999999</v>
       </c>
       <c r="G18">
-        <v>12.2194</v>
+        <v>5.7055999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>12.230700000000001</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>61.433300000000003</v>
+        <v>13.3551</v>
       </c>
       <c r="G19">
-        <v>24.942699999999999</v>
+        <v>14.6106</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>-3.1762000000000001</v>
+        <v>-3.7027999999999999</v>
       </c>
       <c r="F20">
-        <v>42.6265</v>
+        <v>27.255500000000001</v>
       </c>
       <c r="G20">
-        <v>23.130800000000001</v>
+        <v>11.110799999999999</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8195,13 +7283,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.76270000000000004</v>
       </c>
       <c r="F22">
-        <v>1.9496</v>
+        <v>2.4255</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1.3216000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7306,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.72070000000000001</v>
       </c>
       <c r="F23">
-        <v>1.6688000000000001</v>
+        <v>1.5089999999999999</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>0.61370000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8241,13 +7329,13 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>0.45829999999999999</v>
+        <v>0.75139999999999996</v>
       </c>
       <c r="F24">
-        <v>3.8898999999999999</v>
+        <v>1.9189000000000001</v>
       </c>
       <c r="G24">
-        <v>3.032</v>
+        <v>1.2485999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>-1.6879</v>
+        <v>2.7016</v>
       </c>
       <c r="F25">
-        <v>63.305999999999997</v>
+        <v>4.0919999999999996</v>
       </c>
       <c r="G25">
-        <v>50.4649</v>
+        <v>35.709899999999998</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>-1.8727</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F26">
-        <v>11.662000000000001</v>
+        <v>8.2457999999999991</v>
       </c>
       <c r="G26">
-        <v>23.3337</v>
+        <v>3.9060000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>13.2614</v>
+        <v>11.952400000000001</v>
       </c>
       <c r="F29">
-        <v>1.8876999999999999</v>
+        <v>11.952400000000001</v>
       </c>
       <c r="G29">
-        <v>0.21709999999999999</v>
+        <v>2.3258999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7429,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>9.6968999999999994</v>
+        <v>30.228200000000001</v>
       </c>
       <c r="F30">
-        <v>9.8062000000000005</v>
+        <v>8.9684000000000008</v>
       </c>
       <c r="G30">
-        <v>3.1705000000000001</v>
+        <v>1.8367</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,13 +7452,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>11.649900000000001</v>
+        <v>26.2316</v>
       </c>
       <c r="F31">
-        <v>3.7254</v>
+        <v>0.90429999999999999</v>
       </c>
       <c r="G31">
-        <v>6.0811999999999999</v>
+        <v>3.4525000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>12.2293</v>
+        <v>21.839500000000001</v>
       </c>
       <c r="F32">
-        <v>0.94810000000000005</v>
+        <v>0.7994</v>
       </c>
       <c r="G32">
-        <v>4.6520000000000001</v>
+        <v>3.2963</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>12.5162</v>
+        <v>18.7867</v>
       </c>
       <c r="F33">
-        <v>2.7187000000000001</v>
+        <v>2.3940000000000001</v>
       </c>
       <c r="G33">
-        <v>1.0156000000000001</v>
+        <v>4.1786000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>5.6441999999999997</v>
+        <v>3.3712</v>
       </c>
       <c r="F35">
-        <v>5.6441999999999997</v>
+        <v>0.61570000000000003</v>
       </c>
       <c r="G35">
-        <v>1.5902000000000001</v>
+        <v>4.3269000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>12.847300000000001</v>
+        <v>16.232099999999999</v>
       </c>
       <c r="F36">
-        <v>12.8005</v>
+        <v>4.6708999999999996</v>
       </c>
       <c r="G36">
-        <v>0.54349999999999998</v>
+        <v>2.8043999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8479,13 +7567,13 @@
         <v>8</v>
       </c>
       <c r="E37">
-        <v>10.454700000000001</v>
+        <v>30.213899999999999</v>
       </c>
       <c r="F37">
-        <v>15.8614</v>
+        <v>9.1442999999999994</v>
       </c>
       <c r="G37">
-        <v>0.79569999999999996</v>
+        <v>4.9793000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>16.051400000000001</v>
+        <v>31.586500000000001</v>
       </c>
       <c r="F38">
-        <v>22.700700000000001</v>
+        <v>24.207999999999998</v>
       </c>
       <c r="G38">
-        <v>3.2416999999999998</v>
+        <v>2.9344000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>15.5762</v>
+        <v>24.031500000000001</v>
       </c>
       <c r="F39">
-        <v>1.0969</v>
+        <v>3.0455999999999999</v>
       </c>
       <c r="G39">
-        <v>18.361599999999999</v>
+        <v>2.2132999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8548,13 +7636,13 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2.7599</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1.3629</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>2.2035</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>7.5476999999999999</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>2.4821</v>
       </c>
       <c r="G42">
-        <v>6.8838999999999997</v>
+        <v>2.7709999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>10.8827</v>
+        <v>15.053599999999999</v>
       </c>
       <c r="F43">
-        <v>4.3000999999999996</v>
+        <v>2.5268000000000002</v>
       </c>
       <c r="G43">
-        <v>1.9446000000000001</v>
+        <v>4.6219999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>15.3573</v>
+        <v>30.5002</v>
       </c>
       <c r="F44">
-        <v>19.654399999999999</v>
+        <v>6.6894999999999998</v>
       </c>
       <c r="G44">
-        <v>26.616199999999999</v>
+        <v>12.063499999999999</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>16.158799999999999</v>
+        <v>31.707699999999999</v>
       </c>
       <c r="F45">
-        <v>27.836600000000001</v>
+        <v>1.7427999999999999</v>
       </c>
       <c r="G45">
-        <v>18.257000000000001</v>
+        <v>3.7273000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8663,13 +7751,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>3.4207999999999998</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1.3398000000000001</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>2.1347999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8686,13 +7774,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>4.9954999999999998</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1.0542</v>
       </c>
       <c r="G48">
-        <v>1.7171000000000001</v>
+        <v>1.5710999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>1.5734999999999999</v>
+        <v>6.6468999999999996</v>
       </c>
       <c r="F49">
-        <v>1.5734999999999999</v>
+        <v>1.9594</v>
       </c>
       <c r="G49">
-        <v>3.6619999999999999</v>
+        <v>1.4433</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>10.470499999999999</v>
+        <v>15.838100000000001</v>
       </c>
       <c r="F50">
-        <v>7.9917999999999996</v>
+        <v>94.306399999999996</v>
       </c>
       <c r="G50">
-        <v>44.195099999999996</v>
+        <v>37.665199999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>9.7014999999999993</v>
+        <v>24.324300000000001</v>
       </c>
       <c r="F51">
-        <v>1.7801</v>
+        <v>46.541400000000003</v>
       </c>
       <c r="G51">
-        <v>32.2425</v>
+        <v>10.0808</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>13.2614</v>
+        <v>11.952400000000001</v>
       </c>
       <c r="F54">
-        <v>1.8876999999999999</v>
+        <v>11.952400000000001</v>
       </c>
       <c r="G54">
-        <v>0.21709999999999999</v>
+        <v>2.3431999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>11.326700000000001</v>
+        <v>30.371400000000001</v>
       </c>
       <c r="F55">
-        <v>11.436</v>
+        <v>9.1115999999999993</v>
       </c>
       <c r="G55">
-        <v>1.923</v>
+        <v>2.7829999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>40</v>
+        <v>48.367100000000001</v>
       </c>
       <c r="F56">
-        <v>9.5740999999999996</v>
+        <v>5.4191000000000003</v>
       </c>
       <c r="G56">
-        <v>1.5264</v>
+        <v>3.8233999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>60.003700000000002</v>
+        <v>65.147000000000006</v>
       </c>
       <c r="F57">
-        <v>0.55549999999999999</v>
+        <v>5.7813999999999997</v>
       </c>
       <c r="G57">
-        <v>1.8740000000000001</v>
+        <v>1.8925000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>77.846299999999999</v>
+        <v>76.605099999999993</v>
       </c>
       <c r="F58">
-        <v>4.8650000000000002</v>
+        <v>10.654500000000001</v>
       </c>
       <c r="G58">
-        <v>0.23069999999999999</v>
+        <v>4.7366999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>5.6441999999999997</v>
+        <v>3.3712</v>
       </c>
       <c r="F60">
-        <v>5.6441999999999997</v>
+        <v>0.61570000000000003</v>
       </c>
       <c r="G60">
-        <v>1.5902000000000001</v>
+        <v>4.3269000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>12.847300000000001</v>
+        <v>16.232099999999999</v>
       </c>
       <c r="F61">
-        <v>12.8005</v>
+        <v>4.6708999999999996</v>
       </c>
       <c r="G61">
-        <v>0.54349999999999998</v>
+        <v>2.8043999999999998</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>10.454700000000001</v>
+        <v>30.213899999999999</v>
       </c>
       <c r="F62">
-        <v>15.8614</v>
+        <v>9.1442999999999994</v>
       </c>
       <c r="G62">
-        <v>0.79569999999999996</v>
+        <v>4.9793000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>38.173999999999999</v>
+        <v>45.392499999999998</v>
       </c>
       <c r="F63">
-        <v>5.0109000000000004</v>
+        <v>13.8184</v>
       </c>
       <c r="G63">
-        <v>6.3003</v>
+        <v>9.2432999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>61.310600000000001</v>
+        <v>64.805499999999995</v>
       </c>
       <c r="F64">
-        <v>14.902100000000001</v>
+        <v>22.476800000000001</v>
       </c>
       <c r="G64">
-        <v>8.1167999999999996</v>
+        <v>2.0059999999999998</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9016,13 +8104,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>2.7599</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1.3629</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>2.2035</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>7.5476999999999999</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>2.4821</v>
       </c>
       <c r="G67">
-        <v>6.8838999999999997</v>
+        <v>2.7709999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>10.8827</v>
+        <v>15.053599999999999</v>
       </c>
       <c r="F68">
-        <v>4.3000999999999996</v>
+        <v>2.5268000000000002</v>
       </c>
       <c r="G68">
-        <v>1.9446000000000001</v>
+        <v>4.6219999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>26.523900000000001</v>
+        <v>30.5002</v>
       </c>
       <c r="F69">
-        <v>23.739000000000001</v>
+        <v>8.8232999999999997</v>
       </c>
       <c r="G69">
-        <v>16.110499999999998</v>
+        <v>8.8797999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>24.443300000000001</v>
+        <v>44.028300000000002</v>
       </c>
       <c r="F70">
-        <v>33.001899999999999</v>
+        <v>33.578000000000003</v>
       </c>
       <c r="G70">
-        <v>16.8432</v>
+        <v>5.2335000000000003</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8219,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>3.4207999999999998</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>1.3398000000000001</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>2.1347999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8242,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>4.9954999999999998</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>1.0542</v>
       </c>
       <c r="G73">
-        <v>1.7171000000000001</v>
+        <v>1.5710999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>1.5734999999999999</v>
+        <v>6.6468999999999996</v>
       </c>
       <c r="F74">
-        <v>1.5734999999999999</v>
+        <v>1.9594</v>
       </c>
       <c r="G74">
-        <v>3.6619999999999999</v>
+        <v>1.4433</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>8.6221999999999994</v>
+        <v>15.9907</v>
       </c>
       <c r="F75">
-        <v>2.4939</v>
+        <v>12.3911</v>
       </c>
       <c r="G75">
-        <v>49.9315</v>
+        <v>40.655299999999997</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>14.291700000000001</v>
+        <v>29.731000000000002</v>
       </c>
       <c r="F76">
-        <v>6.7023000000000001</v>
+        <v>27.028300000000002</v>
       </c>
       <c r="G76">
-        <v>24.596</v>
+        <v>3.6023000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9257,7 +8345,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>2.0199999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9280,7 +8368,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>3.9342999999999999</v>
+        <v>4.1939000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>27.0684</v>
+        <v>28.2545</v>
       </c>
       <c r="F81">
-        <v>4.4432</v>
+        <v>7.4649999999999999</v>
       </c>
       <c r="G81">
-        <v>5.7645999999999997</v>
+        <v>6.9352</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>54.4985</v>
+        <v>55.442999999999998</v>
       </c>
       <c r="F82">
-        <v>1.7824</v>
+        <v>7.4314</v>
       </c>
       <c r="G82">
-        <v>1.4715</v>
+        <v>1.2806999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>74.558700000000002</v>
+        <v>72.018100000000004</v>
       </c>
       <c r="F83">
-        <v>5.8056999999999999</v>
+        <v>13.721</v>
       </c>
       <c r="G83">
-        <v>0.88129999999999997</v>
+        <v>3.7614000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>31.691500000000001</v>
+        <v>24.593800000000002</v>
       </c>
       <c r="F88">
-        <v>8.5687999999999995</v>
+        <v>27.963999999999999</v>
       </c>
       <c r="G88">
-        <v>9.1980000000000004</v>
+        <v>9.5589999999999993</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>53.721400000000003</v>
+        <v>55.457999999999998</v>
       </c>
       <c r="F89">
-        <v>16.9374</v>
+        <v>31.372699999999998</v>
       </c>
       <c r="G89">
-        <v>1.2712000000000001</v>
+        <v>0.46810000000000002</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>8.9197000000000006</v>
+        <v>-1.2281</v>
       </c>
       <c r="F94">
-        <v>18.812200000000001</v>
+        <v>10.2683</v>
       </c>
       <c r="G94">
-        <v>21.910599999999999</v>
+        <v>16.662199999999999</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>10.476100000000001</v>
+        <v>15.8103</v>
       </c>
       <c r="F95">
-        <v>42.1678</v>
+        <v>46.937399999999997</v>
       </c>
       <c r="G95">
-        <v>22.694900000000001</v>
+        <v>8.0973000000000006</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>0.31190000000000001</v>
+        <v>-0.32890000000000003</v>
       </c>
       <c r="F100">
-        <v>6.4145000000000003</v>
+        <v>1.7988</v>
       </c>
       <c r="G100">
-        <v>8.2644000000000002</v>
+        <v>53.256500000000003</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>0.1547</v>
+        <v>-0.49340000000000001</v>
       </c>
       <c r="F101">
-        <v>7.9634999999999998</v>
+        <v>28.077999999999999</v>
       </c>
       <c r="G101">
-        <v>24.325700000000001</v>
+        <v>42.998100000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>